<commit_message>
Add more stuff, still a ways off
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB74A86-F215-4893-9D7D-FA549363F720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFF8098-038F-4933-9D47-EB2D5BDC339D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3874" uniqueCount="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3903" uniqueCount="1134">
   <si>
     <t># Name</t>
   </si>
@@ -3408,6 +3408,36 @@
   </si>
   <si>
     <t>F,&amp;=A/X,&amp;=Y,G=3</t>
+  </si>
+  <si>
+    <t>A=3,I=1,&amp;=H,&amp;=Y,J=1,&amp;=I,&amp;=B</t>
+  </si>
+  <si>
+    <t>A=3,N=1,&amp;R=1,&amp;=B</t>
+  </si>
+  <si>
+    <t>A=2,N=2,&amp;B=2</t>
+  </si>
+  <si>
+    <t>A=2,B=2,&amp;=T,%=S</t>
+  </si>
+  <si>
+    <t>C=1,R=1,&amp;=B</t>
+  </si>
+  <si>
+    <t>D=2,R=1&amp;=B</t>
+  </si>
+  <si>
+    <t>D=2,K=1,&amp;=H,&amp;=Y</t>
+  </si>
+  <si>
+    <t>Z,&amp;=C,&amp;=Y,D=2,E=1,&amp;=O</t>
+  </si>
+  <si>
+    <t>D=3,P,&amp;=A,&amp;=H</t>
+  </si>
+  <si>
+    <t>A=2/Z,&amp;=Y</t>
   </si>
 </sst>
 </file>
@@ -3838,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A364" workbookViewId="0">
-      <selection activeCell="E378" sqref="E378"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3848,7 +3878,9 @@
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="7" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.5703125" customWidth="1"/>
+    <col min="6" max="6" width="115.7109375" customWidth="1"/>
+    <col min="7" max="7" width="81.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -4001,7 +4033,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>48</v>
+        <v>1124</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4039,7 +4071,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>48</v>
+        <v>1125</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
@@ -4077,7 +4109,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>1126</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4153,7 +4185,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>48</v>
+        <v>1127</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4419,7 +4451,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>1128</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -4495,7 +4527,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>48</v>
+        <v>1131</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4608,9 +4640,7 @@
       <c r="C21">
         <v>7</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
         <v>48</v>
       </c>
@@ -4761,7 +4791,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>48</v>
+        <v>1129</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -4951,7 +4981,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>48</v>
+        <v>1130</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5617,7 +5647,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>48</v>
+        <v>1132</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5780,7 +5810,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>48</v>
+        <v>1133</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Move &=A|B|Y to $
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CAC55D-E7D4-4F51-9A34-3C5565454703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5711A60-A500-4130-8E22-31BAA1E11128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4079" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3950" uniqueCount="1141">
   <si>
     <t># Name</t>
   </si>
@@ -3380,82 +3380,85 @@
     <t>;N=Fountain of Souls</t>
   </si>
   <si>
-    <t>D=1/P,&amp;=4,&amp;=L,&amp;=Y,&amp;=W,&amp;=C</t>
-  </si>
-  <si>
-    <t>D=1/P,&amp;=Y,&amp;=W,&amp;=C</t>
-  </si>
-  <si>
     <t>A=1/C=1</t>
   </si>
   <si>
-    <t>A=1/P,&amp;=A</t>
-  </si>
-  <si>
-    <t>D=1/F,&amp;=A,&amp;=C</t>
-  </si>
-  <si>
-    <t>A=1/L=1,&amp;=A</t>
-  </si>
-  <si>
-    <t>A=1,H,&amp;=H,&amp;=Y,&amp;=4,&amp;=L</t>
-  </si>
-  <si>
     <t>Gain 1$. You may cast any player's prepped spell. That spell deals 1 less damage, minimum 1.</t>
   </si>
   <si>
     <t>The next time you focus or open a breach this turn, it costs 3$ less.#OR#Destroy this. Deal 1 damage.</t>
   </si>
   <si>
-    <t>F,&amp;=A/X,&amp;=Y,G=3</t>
-  </si>
-  <si>
-    <t>A=3,I=1,&amp;=H,&amp;=Y,J=1,&amp;=I,&amp;=B</t>
-  </si>
-  <si>
-    <t>A=3,N=1,&amp;R=1,&amp;=B</t>
-  </si>
-  <si>
     <t>A=2,N=2,&amp;B=2</t>
   </si>
   <si>
     <t>A=2,B=2,&amp;=T,%=S</t>
   </si>
   <si>
-    <t>C=1,R=1,&amp;=B</t>
-  </si>
-  <si>
-    <t>D=2,R=1&amp;=B</t>
-  </si>
-  <si>
-    <t>D=2,K=1,&amp;=H,&amp;=Y</t>
-  </si>
-  <si>
-    <t>Z,&amp;=C,&amp;=Y,D=2,E=1,&amp;=O</t>
-  </si>
-  <si>
-    <t>D=3,P,&amp;=A,&amp;=H</t>
-  </si>
-  <si>
-    <t>A=2/Z,&amp;=Y</t>
-  </si>
-  <si>
-    <t>A=2,Q=1,&amp;=H,&amp;=Y,B=1,&amp;=I</t>
-  </si>
-  <si>
     <t>A=2,B=1,&amp;=N</t>
   </si>
   <si>
-    <t>F,&amp;=A/X,&amp;=Y,L=3,&amp;=Y</t>
-  </si>
-  <si>
-    <t>D=5,X,&amp;=H,&amp;=Y,G=4,&amp;=I</t>
-  </si>
-  <si>
-    <t>D=4/D=2,K=1,&amp;=H,&amp;=B</t>
-  </si>
-  <si>
     <t>A=2/K=1</t>
+  </si>
+  <si>
+    <t>A=3,I=1,&amp;=H,$=Y,J=1,$=B,&amp;=I,$=Y</t>
+  </si>
+  <si>
+    <t>D=3,P,$=A,&amp;=H</t>
+  </si>
+  <si>
+    <t>A=1/L=1,$=A</t>
+  </si>
+  <si>
+    <t>A=1/P,$=A</t>
+  </si>
+  <si>
+    <t>D=1/F,$=A,&amp;=C</t>
+  </si>
+  <si>
+    <t>A=3,N=1,&amp;R=1,$=B</t>
+  </si>
+  <si>
+    <t>C=1,R=1,$=B</t>
+  </si>
+  <si>
+    <t>D=2,R=1$=B</t>
+  </si>
+  <si>
+    <t>D=4/D=2,K=1,&amp;=H,$=B</t>
+  </si>
+  <si>
+    <t>F,$=A/X,$=Y,G=3</t>
+  </si>
+  <si>
+    <t>Z=0,&amp;=C,$=Y,D=2,E=1,&amp;=O</t>
+  </si>
+  <si>
+    <t>D=2,K=1,&amp;=H,$=Y</t>
+  </si>
+  <si>
+    <t>A=2/Z=0,$=Y</t>
+  </si>
+  <si>
+    <t>A=2,Q=1,&amp;=H,$=Y,B=1,&amp;=I,$=Y</t>
+  </si>
+  <si>
+    <t>F,$=A/X,$=Y,L=3,$=Y</t>
+  </si>
+  <si>
+    <t>D=5,X,&amp;=H,$=Y,G=4,&amp;=I,$=Y</t>
+  </si>
+  <si>
+    <t>D=3,I=1,&amp;=H,$=Y,Z=1,&amp;=I,$=Y</t>
+  </si>
+  <si>
+    <t>D=1/P,$=Y,&amp;=W,&amp;=C</t>
+  </si>
+  <si>
+    <t>D=1/P,&amp;=4,&amp;=L,$=Y,&amp;=W,&amp;=C</t>
+  </si>
+  <si>
+    <t>A=1,H,&amp;=H,$=Y,&amp;=4,&amp;=L</t>
   </si>
 </sst>
 </file>
@@ -3886,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,7 +4054,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4089,7 +4092,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
@@ -4127,7 +4130,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1126</v>
+        <v>1117</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4203,7 +4206,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1127</v>
+        <v>1118</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4399,7 +4402,7 @@
         <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1122</v>
+        <v>1116</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>44</v>
@@ -4431,7 +4434,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1123</v>
+        <v>1130</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>48</v>
@@ -4469,7 +4472,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -4809,7 +4812,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -4999,7 +5002,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5665,7 +5668,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1132</v>
+        <v>1122</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5978,7 +5981,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1135</v>
+        <v>1119</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6206,7 +6209,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>48</v>
@@ -6358,7 +6361,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>48</v>
@@ -6434,7 +6437,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1138</v>
+        <v>1129</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6586,7 +6589,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>48</v>
+        <v>1137</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6843,7 +6846,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1139</v>
+        <v>1120</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -15714,7 +15717,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1115</v>
+        <v>1138</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>48</v>
@@ -17598,7 +17601,7 @@
         <v>0</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>1119</v>
+        <v>1123</v>
       </c>
       <c r="E376" s="1" t="s">
         <v>48</v>
@@ -17712,7 +17715,7 @@
         <v>0</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1114</v>
+        <v>1139</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>48</v>
@@ -17902,7 +17905,7 @@
         <v>0</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1117</v>
+        <v>1124</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>48</v>
@@ -18130,7 +18133,7 @@
         <v>0</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>1118</v>
+        <v>1125</v>
       </c>
       <c r="E390" s="1" t="s">
         <v>48</v>
@@ -18320,7 +18323,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1120</v>
+        <v>1140</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>48</v>
@@ -18434,7 +18437,7 @@
         <v>0</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="E398" s="1" t="s">
         <v>48</v>
@@ -18706,7 +18709,7 @@
         <v>48</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>1121</v>
+        <v>1115</v>
       </c>
       <c r="G405" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Merge B and E into A and D
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074346DE-D6D0-468A-85A6-CAF05D8D1C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB92F57-BDE4-4E5E-88B8-3D23E541376A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4073" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3872" uniqueCount="1147">
   <si>
     <t># Name</t>
   </si>
@@ -3389,15 +3389,6 @@
     <t>The next time you focus or open a breach this turn, it costs 3$ less.#OR#Destroy this. Deal 1 damage.</t>
   </si>
   <si>
-    <t>A=2,N=2,&amp;B=2</t>
-  </si>
-  <si>
-    <t>A=2,B=2,&amp;=T,%=S</t>
-  </si>
-  <si>
-    <t>A=2,B=1,&amp;=N</t>
-  </si>
-  <si>
     <t>D=3,P,$=A,&amp;=H</t>
   </si>
   <si>
@@ -3425,15 +3416,9 @@
     <t>F,$=A/X,$=C,G=3</t>
   </si>
   <si>
-    <t>F=0,&amp;=C,$=C,D=2,E=1,&amp;=O</t>
-  </si>
-  <si>
     <t>A=2/F=0,$=C</t>
   </si>
   <si>
-    <t>A=2,Q=1,&amp;=H,$=C,B=1,&amp;=I,$=C</t>
-  </si>
-  <si>
     <t>F,$=A/X,$=C,L=3,$=C</t>
   </si>
   <si>
@@ -3467,9 +3452,6 @@
     <t>A=2/K=1,$=E</t>
   </si>
   <si>
-    <t>D=1,E=1,&amp;=N;L</t>
-  </si>
-  <si>
     <t>A=2/I=1,$=E,C=2,&amp;=I,$=C</t>
   </si>
   <si>
@@ -3477,6 +3459,24 @@
   </si>
   <si>
     <t>C=1/C=-2,&amp;=H,$=C,A=5,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>A=2,N=2,&amp;A=+2</t>
+  </si>
+  <si>
+    <t>A=2,A=+2,&amp;=T,%=S</t>
+  </si>
+  <si>
+    <t>A=2,Q=1,&amp;=H,$=C,A=+1,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>A=2,A=+1,&amp;=N</t>
+  </si>
+  <si>
+    <t>F=0,&amp;=C,$=C,D=2,D=+1,&amp;=O</t>
+  </si>
+  <si>
+    <t>D=1,D=+1,&amp;=N;L</t>
   </si>
 </sst>
 </file>
@@ -3907,8 +3907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4072,7 +4072,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1138</v>
+        <v>1133</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4110,7 +4110,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
@@ -4148,7 +4148,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1117</v>
+        <v>1141</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4224,7 +4224,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1118</v>
+        <v>1142</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4452,7 +4452,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>48</v>
@@ -4490,7 +4490,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -4566,7 +4566,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1129</v>
+        <v>1145</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4830,7 +4830,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -5020,7 +5020,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1140</v>
+        <v>1135</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5686,7 +5686,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5849,7 +5849,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>
@@ -5887,7 +5887,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1131</v>
+        <v>1143</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>48</v>
@@ -5999,7 +5999,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1119</v>
+        <v>1144</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6227,7 +6227,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1132</v>
+        <v>1127</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>48</v>
@@ -6379,7 +6379,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1133</v>
+        <v>1128</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>48</v>
@@ -6455,7 +6455,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1141</v>
+        <v>1136</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6607,7 +6607,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1139</v>
+        <v>1134</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6721,7 +6721,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>143</v>
@@ -6864,7 +6864,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1142</v>
+        <v>1137</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -7016,7 +7016,7 @@
         <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>246</v>
@@ -7092,7 +7092,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1143</v>
+        <v>1146</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>246</v>
@@ -7235,7 +7235,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>48</v>
@@ -7273,7 +7273,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>48</v>
@@ -7349,7 +7349,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>48</v>
@@ -15735,7 +15735,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>48</v>
@@ -17619,7 +17619,7 @@
         <v>0</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="E376" s="1" t="s">
         <v>48</v>
@@ -17733,7 +17733,7 @@
         <v>0</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1136</v>
+        <v>1131</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>48</v>
@@ -17923,7 +17923,7 @@
         <v>0</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>48</v>
@@ -18151,7 +18151,7 @@
         <v>0</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="E390" s="1" t="s">
         <v>48</v>
@@ -18341,7 +18341,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1137</v>
+        <v>1132</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add more params and a runtime checker
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDCF3E2-EC3E-48EA-B446-74FCA8C9B7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE434B-8067-44EF-A87E-CB23E2381F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3935" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4224" uniqueCount="1166">
   <si>
     <t># Name</t>
   </si>
@@ -3338,9 +3338,6 @@
     <t>A=2</t>
   </si>
   <si>
-    <t>A=1,X+2</t>
-  </si>
-  <si>
     <t>A=2,O=1</t>
   </si>
   <si>
@@ -3404,9 +3401,6 @@
     <t>C=1,R=1,$=B</t>
   </si>
   <si>
-    <t>D=2,R=1$=B</t>
-  </si>
-  <si>
     <t>D=2,A=1;L</t>
   </si>
   <si>
@@ -3434,18 +3428,6 @@
     <t>A=1,H,&amp;=H,$=C,&amp;=4,&amp;=L</t>
   </si>
   <si>
-    <t>A=3,I=1,&amp;=H,$=C,$=E,J=1,$=B,&amp;=I,$=C</t>
-  </si>
-  <si>
-    <t>D=3,I=1,&amp;=H,$=C,$=E,Z=0,&amp;=I,$=C</t>
-  </si>
-  <si>
-    <t>D=2,K=1,&amp;=H,$=C,$=E</t>
-  </si>
-  <si>
-    <t>D=4/D=2,K=1,&amp;=H,$=B,$=E</t>
-  </si>
-  <si>
     <t>A=3/A=2,D=1</t>
   </si>
   <si>
@@ -3482,13 +3464,76 @@
     <t>Cast: Deal 2 damage. If you have two or more other prepped spells, deal 1 additional damage.</t>
   </si>
   <si>
-    <t>A=2/I=1,$=C,$=E,C=2,&amp;=I,$=C</t>
-  </si>
-  <si>
-    <t>A=2/K=1,$=C,$=E</t>
-  </si>
-  <si>
-    <t>C=1,K=1,&amp;=H,$=C,$=G</t>
+    <t>D=5,J=1,$=D</t>
+  </si>
+  <si>
+    <t>D=7,&amp;=D;D</t>
+  </si>
+  <si>
+    <t>I=1,$=A,&amp;=C,D=4,&amp;=I</t>
+  </si>
+  <si>
+    <t>D=2,F=3,$=A</t>
+  </si>
+  <si>
+    <t>C=1,Z=0,$=B</t>
+  </si>
+  <si>
+    <t>A=2,J=1,$=B</t>
+  </si>
+  <si>
+    <t>A=2/X,$=C,A=3</t>
+  </si>
+  <si>
+    <t>G=2/L=2,$=A</t>
+  </si>
+  <si>
+    <t>D=2;E</t>
+  </si>
+  <si>
+    <t>D=1,A=1,&amp;=T,%=C;E</t>
+  </si>
+  <si>
+    <t>D=1,F,$=B;E</t>
+  </si>
+  <si>
+    <t>A=1,X,&amp;=H,$=C,A=+2,&amp;=I</t>
+  </si>
+  <si>
+    <t>F=0,$=C/X,$=C,C=1</t>
+  </si>
+  <si>
+    <t>C=1,&amp;=C</t>
+  </si>
+  <si>
+    <t>D=1/J=1,$=B,&amp;=C</t>
+  </si>
+  <si>
+    <t>A=3,I=1,&amp;=H,$=C,$=J,$=E,J=1,$=B,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>D=2,R=1,$=B</t>
+  </si>
+  <si>
+    <t>D=2,K=1,&amp;=H,$=C,$=J,$=E</t>
+  </si>
+  <si>
+    <t>C=1,K=1,&amp;=H,$=C,$=J,$=H</t>
+  </si>
+  <si>
+    <t>D=4/D=2,K=1,&amp;=H,$=B,$=J,$=E</t>
+  </si>
+  <si>
+    <t>D=3,I=1,&amp;=H,$=C,$=J,$=E,Z=0,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>A=2/K=1,$=C,$=J,$=E</t>
+  </si>
+  <si>
+    <t>A=2/I=1,$=C,$=J,$=E,C=2,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>K=1,$=A,$=K,$=I/X,$=C,L=2,$=C</t>
   </si>
 </sst>
 </file>
@@ -3919,8 +3964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4084,7 +4129,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1132</v>
+        <v>1157</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4122,7 +4167,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
@@ -4160,7 +4205,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1138</v>
+        <v>1132</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4236,7 +4281,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1139</v>
+        <v>1133</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4432,7 +4477,7 @@
         <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>44</v>
@@ -4464,7 +4509,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>48</v>
@@ -4502,7 +4547,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -4578,7 +4623,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1142</v>
+        <v>1136</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4842,7 +4887,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1122</v>
+        <v>1158</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -5032,7 +5077,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1134</v>
+        <v>1159</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5175,7 +5220,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1150</v>
+        <v>1160</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>48</v>
@@ -5288,7 +5333,9 @@
       <c r="C37">
         <v>8</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>1142</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>48</v>
       </c>
@@ -5658,7 +5705,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>48</v>
+        <v>1143</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>143</v>
@@ -5696,7 +5743,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5859,7 +5906,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>
@@ -5897,7 +5944,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1140</v>
+        <v>1134</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>48</v>
@@ -6009,7 +6056,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6237,7 +6284,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>48</v>
@@ -6389,7 +6436,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>48</v>
@@ -6465,7 +6512,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1135</v>
+        <v>1161</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6617,7 +6664,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1133</v>
+        <v>1162</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6731,7 +6778,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>143</v>
@@ -6874,7 +6921,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1149</v>
+        <v>1163</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -7026,7 +7073,7 @@
         <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>246</v>
@@ -7102,7 +7149,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1143</v>
+        <v>1137</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>246</v>
@@ -7245,7 +7292,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1148</v>
+        <v>1164</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>48</v>
@@ -7283,7 +7330,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1136</v>
+        <v>1130</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>48</v>
@@ -7359,7 +7406,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1137</v>
+        <v>1131</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>48</v>
@@ -7435,7 +7482,7 @@
         <v>6</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1144</v>
+        <v>1138</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>48</v>
@@ -7473,7 +7520,7 @@
         <v>5</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1145</v>
+        <v>1139</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>48</v>
@@ -7788,7 +7835,7 @@
         <v>6</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>48</v>
@@ -7864,7 +7911,7 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1146</v>
+        <v>1140</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>48</v>
@@ -7946,7 +7993,7 @@
         <v>48</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1147</v>
+        <v>1141</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>310</v>
@@ -8016,7 +8063,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>48</v>
+        <v>1144</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>48</v>
@@ -8159,7 +8206,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>48</v>
+        <v>1145</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>48</v>
@@ -8378,7 +8425,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>48</v>
+        <v>1146</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>48</v>
@@ -8445,7 +8492,7 @@
         <v>3</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>48</v>
@@ -8664,7 +8711,7 @@
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>48</v>
+        <v>1147</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>48</v>
@@ -8702,7 +8749,7 @@
         <v>6</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>48</v>
@@ -10273,7 +10320,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>48</v>
+        <v>1148</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>48</v>
@@ -10348,9 +10395,7 @@
       <c r="C175">
         <v>5</v>
       </c>
-      <c r="D175" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D175" s="1"/>
       <c r="E175" s="1" t="s">
         <v>48</v>
       </c>
@@ -10682,7 +10727,7 @@
         <v>3</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>48</v>
+        <v>1165</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>48</v>
@@ -10720,7 +10765,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>48</v>
+        <v>1149</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>48</v>
@@ -10901,7 +10946,7 @@
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>48</v>
+        <v>1150</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>530</v>
@@ -11044,7 +11089,7 @@
         <v>4</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>48</v>
+        <v>1151</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>530</v>
@@ -11701,7 +11746,7 @@
         <v>5</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>48</v>
+        <v>1152</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>530</v>
@@ -12530,7 +12575,7 @@
         <v>4</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E235" s="1" t="s">
         <v>48</v>
@@ -13073,7 +13118,7 @@
         <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1100</v>
+        <v>1153</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>48</v>
@@ -13111,7 +13156,7 @@
         <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>48</v>
+        <v>1154</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>48</v>
@@ -14731,7 +14776,7 @@
         <v>0</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E296" s="1" t="s">
         <v>48</v>
@@ -14767,7 +14812,7 @@
         <v>0</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E297" s="1" t="s">
         <v>48</v>
@@ -14803,7 +14848,7 @@
         <v>0</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E298" s="1" t="s">
         <v>48</v>
@@ -14992,7 +15037,7 @@
         <v>2</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E304" s="1" t="s">
         <v>767</v>
@@ -15028,7 +15073,7 @@
         <v>3</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E305" s="1" t="s">
         <v>772</v>
@@ -15064,7 +15109,7 @@
         <v>3</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E306" s="1" t="s">
         <v>772</v>
@@ -15100,7 +15145,7 @@
         <v>6</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E307" s="1" t="s">
         <v>772</v>
@@ -15136,7 +15181,7 @@
         <v>6</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E308" s="1" t="s">
         <v>772</v>
@@ -15172,7 +15217,7 @@
         <v>3</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E309" s="1" t="s">
         <v>786</v>
@@ -15208,7 +15253,7 @@
         <v>3</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E310" s="1" t="s">
         <v>786</v>
@@ -15244,7 +15289,7 @@
         <v>6</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E311" s="1" t="s">
         <v>786</v>
@@ -15280,7 +15325,7 @@
         <v>6</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E312" s="1" t="s">
         <v>786</v>
@@ -15745,7 +15790,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>48</v>
@@ -16411,7 +16456,7 @@
         <v>0</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>1092</v>
+        <v>1155</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>48</v>
@@ -16449,7 +16494,7 @@
         <v>0</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>48</v>
+        <v>1156</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>48</v>
@@ -17629,7 +17674,7 @@
         <v>0</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E376" s="1" t="s">
         <v>48</v>
@@ -17743,7 +17788,7 @@
         <v>0</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>48</v>
@@ -17933,7 +17978,7 @@
         <v>0</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>48</v>
@@ -18161,7 +18206,7 @@
         <v>0</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E390" s="1" t="s">
         <v>48</v>
@@ -18351,7 +18396,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>48</v>
@@ -18465,7 +18510,7 @@
         <v>0</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E398" s="1" t="s">
         <v>48</v>
@@ -18737,7 +18782,7 @@
         <v>48</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G405" s="1" t="s">
         <v>48</v>
@@ -19189,7 +19234,7 @@
         <v>0</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E418" s="1" t="s">
         <v>1060</v>
@@ -19256,7 +19301,7 @@
         <v>3</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E420" s="1" t="s">
         <v>48</v>
@@ -19294,7 +19339,7 @@
         <v>3</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E421" s="1" t="s">
         <v>48</v>
@@ -19332,7 +19377,7 @@
         <v>3</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E422" s="1" t="s">
         <v>48</v>
@@ -19370,7 +19415,7 @@
         <v>4</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E423" s="1" t="s">
         <v>48</v>
@@ -19408,7 +19453,7 @@
         <v>4</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E424" s="1" t="s">
         <v>48</v>
@@ -19446,7 +19491,7 @@
         <v>4</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E425" s="1" t="s">
         <v>48</v>
@@ -19484,7 +19529,7 @@
         <v>5</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E426" s="1" t="s">
         <v>48</v>
@@ -19522,7 +19567,7 @@
         <v>5</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E427" s="1" t="s">
         <v>48</v>
@@ -19560,7 +19605,7 @@
         <v>5</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E428" s="1" t="s">
         <v>48</v>
@@ -19627,7 +19672,7 @@
         <v>0</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E430" s="1" t="s">
         <v>1083</v>
@@ -19694,7 +19739,7 @@
         <v>3</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E432" s="1" t="s">
         <v>1086</v>

</xml_diff>

<commit_message>
Add testing for card codes
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AE434B-8067-44EF-A87E-CB23E2381F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0679438B-93F4-48B4-B4B3-233F7380EC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4224" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="1166">
   <si>
     <t># Name</t>
   </si>
@@ -3383,9 +3383,6 @@
     <t>The next time you focus or open a breach this turn, it costs 3$ less.#OR#Destroy this. Deal 1 damage.</t>
   </si>
   <si>
-    <t>D=3,P,$=A,&amp;=H</t>
-  </si>
-  <si>
     <t>A=1/L=1,$=A</t>
   </si>
   <si>
@@ -3416,9 +3413,6 @@
     <t>D=5,X,&amp;=H,$=C,G=4,&amp;=I,$=C</t>
   </si>
   <si>
-    <t>D=4,M=1,&amp;=H,$=C;D</t>
-  </si>
-  <si>
     <t>D=1/P,$=C,&amp;=W,&amp;=C</t>
   </si>
   <si>
@@ -3437,9 +3431,6 @@
     <t>A=2,N=2,&amp;A=+2</t>
   </si>
   <si>
-    <t>A=2,A=+2,&amp;=T,%=S</t>
-  </si>
-  <si>
     <t>A=2,Q=1,&amp;=H,$=C,A=+1,&amp;=I,$=C</t>
   </si>
   <si>
@@ -3455,9 +3446,6 @@
     <t>D=2,D=+5,&amp;=0-2,$=C</t>
   </si>
   <si>
-    <t>D=3,D=+3,&amp;=+4</t>
-  </si>
-  <si>
     <t>J=2,$=B</t>
   </si>
   <si>
@@ -3470,9 +3458,6 @@
     <t>D=7,&amp;=D;D</t>
   </si>
   <si>
-    <t>I=1,$=A,&amp;=C,D=4,&amp;=I</t>
-  </si>
-  <si>
     <t>D=2,F=3,$=A</t>
   </si>
   <si>
@@ -3497,9 +3482,6 @@
     <t>D=1,F,$=B;E</t>
   </si>
   <si>
-    <t>A=1,X,&amp;=H,$=C,A=+2,&amp;=I</t>
-  </si>
-  <si>
     <t>F=0,$=C/X,$=C,C=1</t>
   </si>
   <si>
@@ -3533,7 +3515,25 @@
     <t>A=2/I=1,$=C,$=J,$=E,C=2,&amp;=I,$=C</t>
   </si>
   <si>
-    <t>K=1,$=A,$=K,$=I/X,$=C,L=2,$=C</t>
+    <t>D=3,P,$=A,&amp;=H,$=C</t>
+  </si>
+  <si>
+    <t>D=3,D=+3,&amp;=+4,$=C</t>
+  </si>
+  <si>
+    <t>A=2,A=+1,&amp;=T,%=S</t>
+  </si>
+  <si>
+    <t>A=1,X,&amp;=H,$=C,A=+2,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>K=1,$=C,$=K,$=I/X,$=C,L=2,$=C</t>
+  </si>
+  <si>
+    <t>D=4,K=1,&amp;=H,$=C,$=J,$=F;D</t>
+  </si>
+  <si>
+    <t>I=1,$==A,$=J,$=E,&amp;=C,D=4,&amp;=I,$=A</t>
   </si>
 </sst>
 </file>
@@ -3964,8 +3964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4129,7 +4129,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1157</v>
+        <v>1151</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4167,7 +4167,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
@@ -4205,7 +4205,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4281,7 +4281,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1133</v>
+        <v>1161</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4509,7 +4509,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>48</v>
@@ -4547,7 +4547,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -4623,7 +4623,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4887,7 +4887,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1158</v>
+        <v>1152</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -5077,7 +5077,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1159</v>
+        <v>1153</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5220,7 +5220,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1160</v>
+        <v>1154</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>48</v>
@@ -5334,7 +5334,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>48</v>
@@ -5705,7 +5705,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>143</v>
@@ -5743,7 +5743,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1115</v>
+        <v>1159</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5906,7 +5906,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>
@@ -5944,7 +5944,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>48</v>
@@ -6056,7 +6056,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6284,7 +6284,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>48</v>
@@ -6436,7 +6436,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>48</v>
@@ -6512,7 +6512,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1161</v>
+        <v>1155</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6664,7 +6664,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1162</v>
+        <v>1156</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6778,7 +6778,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1126</v>
+        <v>1164</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>143</v>
@@ -6815,9 +6815,7 @@
       <c r="C77">
         <v>7</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
         <v>226</v>
       </c>
@@ -6921,7 +6919,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1163</v>
+        <v>1157</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -7073,7 +7071,7 @@
         <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>246</v>
@@ -7149,7 +7147,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>246</v>
@@ -7292,7 +7290,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1164</v>
+        <v>1158</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>48</v>
@@ -7330,7 +7328,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>48</v>
@@ -7406,7 +7404,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>48</v>
@@ -7482,7 +7480,7 @@
         <v>6</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>48</v>
@@ -7520,7 +7518,7 @@
         <v>5</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1139</v>
+        <v>1160</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>48</v>
@@ -7911,7 +7909,7 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>48</v>
@@ -7993,7 +7991,7 @@
         <v>48</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>310</v>
@@ -8063,7 +8061,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1144</v>
+        <v>1165</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>48</v>
@@ -8206,7 +8204,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1145</v>
+        <v>1140</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>48</v>
@@ -8425,7 +8423,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1146</v>
+        <v>1141</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>48</v>
@@ -8711,7 +8709,7 @@
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1147</v>
+        <v>1142</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>48</v>
@@ -10320,7 +10318,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1148</v>
+        <v>1143</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>48</v>
@@ -10727,7 +10725,7 @@
         <v>3</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>48</v>
@@ -10765,7 +10763,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>48</v>
@@ -10946,7 +10944,7 @@
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1150</v>
+        <v>1145</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>530</v>
@@ -11089,7 +11087,7 @@
         <v>4</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1151</v>
+        <v>1146</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>530</v>
@@ -11746,7 +11744,7 @@
         <v>5</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1152</v>
+        <v>1147</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>530</v>
@@ -13118,7 +13116,7 @@
         <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1153</v>
+        <v>1162</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>48</v>
@@ -13156,7 +13154,7 @@
         <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1154</v>
+        <v>1148</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>48</v>
@@ -15790,7 +15788,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>48</v>
@@ -16456,7 +16454,7 @@
         <v>0</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>1155</v>
+        <v>1149</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>48</v>
@@ -16494,7 +16492,7 @@
         <v>0</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>1156</v>
+        <v>1150</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>48</v>
@@ -17674,7 +17672,7 @@
         <v>0</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E376" s="1" t="s">
         <v>48</v>
@@ -17788,7 +17786,7 @@
         <v>0</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>48</v>
@@ -17978,7 +17976,7 @@
         <v>0</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>48</v>
@@ -18206,7 +18204,7 @@
         <v>0</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E390" s="1" t="s">
         <v>48</v>
@@ -18396,7 +18394,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add more codifying stuff
Now with ?=* for the Special section, which tells it to look for the Effect types
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7928D18-F637-41B7-BEE1-270E6EE92200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973DB092-0F0D-4BB3-87FF-116B87348D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3870" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="1170">
   <si>
     <t># Name</t>
   </si>
@@ -3422,9 +3422,6 @@
     <t>A=1,H,&amp;=H,$=C,&amp;=4,&amp;=L</t>
   </si>
   <si>
-    <t>A=3/A=2,D=1</t>
-  </si>
-  <si>
     <t>C=1/C=-2,&amp;=H,$=C,A=5,&amp;=I,$=C</t>
   </si>
   <si>
@@ -3534,6 +3531,21 @@
   </si>
   <si>
     <t>D=3,I=1,&amp;=H,$=C,$=J,$=E,Z=0,$=A,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>D=3,M=!1,&amp;C=1;L</t>
+  </si>
+  <si>
+    <t>A=3/A=2,&amp;&amp;D=1</t>
+  </si>
+  <si>
+    <t>D=3;C</t>
+  </si>
+  <si>
+    <t>D=3;P;&amp;=C;?=D:1</t>
+  </si>
+  <si>
+    <t>X,$=C,K=0-2,$=C,$=J,$=G,J=1,$=C</t>
   </si>
 </sst>
 </file>
@@ -3964,8 +3976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4129,7 +4141,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4205,7 +4217,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4281,7 +4293,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4433,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>48</v>
+        <v>1169</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>48</v>
@@ -4470,9 +4482,7 @@
       <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>48</v>
       </c>
@@ -4623,7 +4633,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4849,7 +4859,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>1167</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>76</v>
@@ -4887,7 +4897,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -4925,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>48</v>
+        <v>1168</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>83</v>
@@ -5077,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5220,7 +5230,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>48</v>
@@ -5334,7 +5344,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>48</v>
@@ -5705,7 +5715,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>143</v>
@@ -5743,7 +5753,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5944,7 +5954,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>48</v>
@@ -6056,7 +6066,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6512,7 +6522,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6664,7 +6674,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6778,7 +6788,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>143</v>
@@ -6919,7 +6929,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -7147,7 +7157,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>246</v>
@@ -7185,7 +7195,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>48</v>
+        <v>1165</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>246</v>
@@ -7290,7 +7300,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>48</v>
@@ -7328,7 +7338,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1128</v>
+        <v>1166</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>48</v>
@@ -7404,7 +7414,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>48</v>
@@ -7480,7 +7490,7 @@
         <v>6</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>48</v>
@@ -7518,7 +7528,7 @@
         <v>5</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>48</v>
@@ -7909,7 +7919,7 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>48</v>
@@ -7991,7 +8001,7 @@
         <v>48</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>310</v>
@@ -8061,7 +8071,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>48</v>
@@ -8204,7 +8214,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>48</v>
@@ -8423,7 +8433,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>48</v>
@@ -8709,7 +8719,7 @@
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>48</v>
@@ -10318,7 +10328,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>48</v>
@@ -10725,7 +10735,7 @@
         <v>3</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>48</v>
@@ -10763,7 +10773,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>48</v>
@@ -10944,7 +10954,7 @@
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>530</v>
@@ -11087,7 +11097,7 @@
         <v>4</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>530</v>
@@ -11744,7 +11754,7 @@
         <v>5</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>530</v>
@@ -13116,7 +13126,7 @@
         <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>48</v>
@@ -13154,7 +13164,7 @@
         <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>48</v>
@@ -16454,7 +16464,7 @@
         <v>0</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>48</v>
@@ -16492,7 +16502,7 @@
         <v>0</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Change X to be "destroy this" always
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973DB092-0F0D-4BB3-87FF-116B87348D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AD458C-3B4A-49FF-BD58-6A59495EC520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3999" uniqueCount="1170">
   <si>
     <t># Name</t>
   </si>
@@ -3401,15 +3401,9 @@
     <t>D=2,A=1;L</t>
   </si>
   <si>
-    <t>F,$=A/X,$=C,G=3</t>
-  </si>
-  <si>
     <t>A=2/F=0,$=C</t>
   </si>
   <si>
-    <t>F,$=A/X,$=C,L=3,$=C</t>
-  </si>
-  <si>
     <t>D=5,X,&amp;=H,$=C,G=4,&amp;=I,$=C</t>
   </si>
   <si>
@@ -3464,9 +3458,6 @@
     <t>A=2,J=1,$=B</t>
   </si>
   <si>
-    <t>A=2/X,$=C,A=3</t>
-  </si>
-  <si>
     <t>G=2/L=2,$=A</t>
   </si>
   <si>
@@ -3479,9 +3470,6 @@
     <t>D=1,F,$=B;E</t>
   </si>
   <si>
-    <t>F=0,$=C/X,$=C,C=1</t>
-  </si>
-  <si>
     <t>C=1,&amp;=C</t>
   </si>
   <si>
@@ -3521,9 +3509,6 @@
     <t>A=1,X,&amp;=H,$=C,A=+2,&amp;=I,$=C</t>
   </si>
   <si>
-    <t>K=1,$=C,$=K,$=I/X,$=C,L=2,$=C</t>
-  </si>
-  <si>
     <t>D=4,K=1,&amp;=H,$=C,$=J,$=F;D</t>
   </si>
   <si>
@@ -3545,7 +3530,22 @@
     <t>D=3;P;&amp;=C;?=D:1</t>
   </si>
   <si>
-    <t>X,$=C,K=0-2,$=C,$=J,$=G,J=1,$=C</t>
+    <t>X,K=0-2,$=C,$=J,$=G,J=1,$=C</t>
+  </si>
+  <si>
+    <t>F,$=A/X,G=3</t>
+  </si>
+  <si>
+    <t>F,$=A/X,L=3,$=C</t>
+  </si>
+  <si>
+    <t>A=2/X,A=3</t>
+  </si>
+  <si>
+    <t>K=1,$=C,$=K,$=I/X,L=2,$=C</t>
+  </si>
+  <si>
+    <t>F=0,$=C/X,C=1</t>
   </si>
 </sst>
 </file>
@@ -3976,8 +3976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4141,7 +4141,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4217,7 +4217,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4293,7 +4293,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4445,7 +4445,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1169</v>
+        <v>1164</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>48</v>
@@ -4519,7 +4519,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1121</v>
+        <v>1165</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>48</v>
@@ -4633,7 +4633,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4859,7 +4859,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>76</v>
@@ -4897,7 +4897,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -4935,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>83</v>
@@ -5087,7 +5087,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5230,7 +5230,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>48</v>
@@ -5344,7 +5344,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>48</v>
@@ -5715,7 +5715,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>143</v>
@@ -5753,7 +5753,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5916,7 +5916,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>
@@ -5954,7 +5954,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>48</v>
@@ -6066,7 +6066,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6294,7 +6294,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1123</v>
+        <v>1166</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>48</v>
@@ -6446,7 +6446,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>48</v>
@@ -6522,7 +6522,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6674,7 +6674,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1164</v>
+        <v>1159</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6788,7 +6788,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>143</v>
@@ -6929,7 +6929,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -7157,7 +7157,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>246</v>
@@ -7195,7 +7195,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1165</v>
+        <v>1160</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>246</v>
@@ -7300,7 +7300,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>48</v>
@@ -7338,7 +7338,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1166</v>
+        <v>1161</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>48</v>
@@ -7414,7 +7414,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>48</v>
@@ -7490,7 +7490,7 @@
         <v>6</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>48</v>
@@ -7528,7 +7528,7 @@
         <v>5</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>48</v>
@@ -7919,7 +7919,7 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>48</v>
@@ -8001,7 +8001,7 @@
         <v>48</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>310</v>
@@ -8071,7 +8071,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>48</v>
@@ -8214,7 +8214,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>48</v>
@@ -8433,7 +8433,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>48</v>
@@ -8719,7 +8719,7 @@
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>48</v>
@@ -10328,7 +10328,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1142</v>
+        <v>1167</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>48</v>
@@ -10735,7 +10735,7 @@
         <v>3</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1161</v>
+        <v>1168</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>48</v>
@@ -10773,7 +10773,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>48</v>
@@ -10954,7 +10954,7 @@
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>530</v>
@@ -11097,7 +11097,7 @@
         <v>4</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>530</v>
@@ -11754,7 +11754,7 @@
         <v>5</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>530</v>
@@ -13126,7 +13126,7 @@
         <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>48</v>
@@ -13164,7 +13164,7 @@
         <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1147</v>
+        <v>1169</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>48</v>
@@ -15798,7 +15798,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>48</v>
@@ -16464,7 +16464,7 @@
         <v>0</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>48</v>
@@ -16502,7 +16502,7 @@
         <v>0</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>48</v>
@@ -17796,7 +17796,7 @@
         <v>0</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>48</v>
@@ -18404,7 +18404,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
More changes to codes
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AD458C-3B4A-49FF-BD58-6A59495EC520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22E8468-97E9-4191-804C-2B74B73FCC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3999" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3869" uniqueCount="1171">
   <si>
     <t># Name</t>
   </si>
@@ -3546,6 +3546,9 @@
   </si>
   <si>
     <t>F=0,$=C/X,C=1</t>
+  </si>
+  <si>
+    <t>D=2,N=2,&amp;D=+2;L</t>
   </si>
 </sst>
 </file>
@@ -3976,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="D252" sqref="D252"/>
+    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="D243" sqref="D243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12840,7 +12843,7 @@
         <v>3</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>48</v>
+        <v>1170</v>
       </c>
       <c r="E242" s="1" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
Completely redo the code handling
There's still some errors; namely, source vs target awareness is not very good and needs to be improved to be per-token, rather than per-context. Currently 24 mismatches, which is fairly good, considering the 22 mismatches with the previous system.
</commit_message>
<xml_diff>
--- a/Player Cards.xlsx
+++ b/Player Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6759C01F-156E-4DE7-A69D-3223A21C5427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04E17E-C2AF-4A68-9097-E0A784B6FD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9B7A286-D4BB-4D76-82A4-94EB548F212D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4070" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3869" uniqueCount="1171">
   <si>
     <t># Name</t>
   </si>
@@ -3371,9 +3371,6 @@
     <t>A=1/L=1,$=A</t>
   </si>
   <si>
-    <t>A=1/P,$=A</t>
-  </si>
-  <si>
     <t>D=1/F,$=A,&amp;=C</t>
   </si>
   <si>
@@ -3386,15 +3383,6 @@
     <t>D=5,X,&amp;=H,$=C,G=4,&amp;=I,$=C</t>
   </si>
   <si>
-    <t>D=1/P,$=C,&amp;=W,&amp;=C</t>
-  </si>
-  <si>
-    <t>D=1/P,&amp;=4,&amp;=L,$=C,&amp;=W,&amp;=C</t>
-  </si>
-  <si>
-    <t>A=1,H,&amp;=H,$=C,&amp;=4,&amp;=L</t>
-  </si>
-  <si>
     <t>A=2,N=2,&amp;A=+2</t>
   </si>
   <si>
@@ -3437,51 +3425,18 @@
     <t>D=2;E</t>
   </si>
   <si>
-    <t>D=1,A=1,&amp;=T,%=C;E</t>
-  </si>
-  <si>
     <t>D=1,F,$=B;E</t>
   </si>
   <si>
     <t>D=1/J=1,$=B,&amp;=C</t>
   </si>
   <si>
-    <t>A=3,I=1,&amp;=H,$=C,$=J,$=E,J=1,$=B,&amp;=I,$=C</t>
-  </si>
-  <si>
-    <t>D=2,K=1,&amp;=H,$=C,$=J,$=E</t>
-  </si>
-  <si>
-    <t>D=4/D=2,K=1,&amp;=H,$=B,$=J,$=E</t>
-  </si>
-  <si>
-    <t>A=2/K=1,$=C,$=J,$=E</t>
-  </si>
-  <si>
-    <t>A=2/I=1,$=C,$=J,$=E,C=2,&amp;=I,$=C</t>
-  </si>
-  <si>
-    <t>D=3,P,$=A,&amp;=H,$=C</t>
-  </si>
-  <si>
     <t>D=3,D=+3,&amp;=+4,$=C</t>
   </si>
   <si>
-    <t>A=2,A=+1,&amp;=T,%=S</t>
-  </si>
-  <si>
     <t>A=1,X,&amp;=H,$=C,A=+2,&amp;=I,$=C</t>
   </si>
   <si>
-    <t>D=4,K=1,&amp;=H,$=C,$=J,$=F;D</t>
-  </si>
-  <si>
-    <t>I=1,$==A,$=J,$=E,&amp;=C,D=4,&amp;=I,$=A</t>
-  </si>
-  <si>
-    <t>D=3,I=1,&amp;=H,$=C,$=J,$=E,Z=0,$=A,&amp;=I,$=C</t>
-  </si>
-  <si>
     <t>A=3/A=2,&amp;&amp;D=1</t>
   </si>
   <si>
@@ -3491,9 +3446,6 @@
     <t>D=3;P;&amp;=C;?=D:1</t>
   </si>
   <si>
-    <t>X,K=0-2,$=C,$=J,$=G,J=1,$=C</t>
-  </si>
-  <si>
     <t>F,$=A/X,G=3</t>
   </si>
   <si>
@@ -3503,9 +3455,6 @@
     <t>A=2/X,A=3</t>
   </si>
   <si>
-    <t>K=1,$=C,$=K,$=I/X,L=2,$=C</t>
-  </si>
-  <si>
     <t>D=2,N=2,&amp;D=+2;L</t>
   </si>
   <si>
@@ -3515,9 +3464,6 @@
     <t>C=1,$=C,C=1,$=B</t>
   </si>
   <si>
-    <t>C=1,$=C,K=1,&amp;=H,$=C,$=J,$=H</t>
-  </si>
-  <si>
     <t>C=1,$=C/C=-2,&amp;=H,$=C,A=5,&amp;=I,$=C</t>
   </si>
   <si>
@@ -3549,6 +3495,60 @@
   </si>
   <si>
     <t>Reverberating Shock</t>
+  </si>
+  <si>
+    <t>D=1/B,$=C,&amp;=W,&amp;=C</t>
+  </si>
+  <si>
+    <t>A=1/B,$=A</t>
+  </si>
+  <si>
+    <t>D=3,B,$=A,&amp;=H,$=C</t>
+  </si>
+  <si>
+    <t>D=1/B,&amp;=4-,$=C,&amp;=W,&amp;=C</t>
+  </si>
+  <si>
+    <t>A=1,H,&amp;=H,$=C,&amp;=4-</t>
+  </si>
+  <si>
+    <t>A=2,A=+1,%=S</t>
+  </si>
+  <si>
+    <t>D=1,A=1,%=C;E</t>
+  </si>
+  <si>
+    <t>A=3,I=1,&amp;=H,$=C,$=E,J=1,$=B,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>X,K=0-2,$=C,$=G,J=1,$=C</t>
+  </si>
+  <si>
+    <t>D=2,K=1,&amp;=H,$=C,$=E</t>
+  </si>
+  <si>
+    <t>C=1,$=C,K=1,&amp;=H,$=C,$=H</t>
+  </si>
+  <si>
+    <t>D=4/D=2,K=1,&amp;=H,$=B,$=E</t>
+  </si>
+  <si>
+    <t>D=3,I=1,&amp;=H,$=C,$=E,Z=0,$=A,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>D=4,K=1,&amp;=H,$=C,$=F;D</t>
+  </si>
+  <si>
+    <t>A=2/K=1,$=C,$=E</t>
+  </si>
+  <si>
+    <t>A=2/I=1,$=C,$=E,C=2,&amp;=I,$=C</t>
+  </si>
+  <si>
+    <t>K=1,$=C,$=I/X,L=2,$=C</t>
+  </si>
+  <si>
+    <t>I=1,$=A,$=E,&amp;=C,D=4,&amp;=I,$=A</t>
   </si>
 </sst>
 </file>
@@ -3979,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD30BF-D2F4-4233-AF09-6D096A2CEE65}">
   <dimension ref="A1:L432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="A195" sqref="A195"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4144,7 +4144,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1136</v>
+        <v>1160</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>48</v>
@@ -4182,7 +4182,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1169</v>
+        <v>1151</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>48</v>
@@ -4220,7 +4220,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>48</v>
@@ -4296,7 +4296,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1143</v>
+        <v>1158</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>48</v>
@@ -4448,7 +4448,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1151</v>
+        <v>1161</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>48</v>
@@ -4522,7 +4522,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1152</v>
+        <v>1136</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>48</v>
@@ -4560,7 +4560,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1158</v>
+        <v>1141</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>48</v>
@@ -4636,7 +4636,7 @@
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>48</v>
@@ -4862,7 +4862,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1149</v>
+        <v>1134</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>76</v>
@@ -4900,7 +4900,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1168</v>
+        <v>1150</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>48</v>
@@ -4938,7 +4938,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1150</v>
+        <v>1135</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>83</v>
@@ -5090,7 +5090,7 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1137</v>
+        <v>1162</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>48</v>
@@ -5233,7 +5233,7 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>1159</v>
+        <v>1163</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>48</v>
@@ -5347,7 +5347,7 @@
         <v>8</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>48</v>
@@ -5718,7 +5718,7 @@
         <v>8</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>143</v>
@@ -5756,7 +5756,7 @@
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1141</v>
+        <v>1155</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>48</v>
@@ -5919,7 +5919,7 @@
         <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>48</v>
@@ -5957,7 +5957,7 @@
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>48</v>
@@ -6069,7 +6069,7 @@
         <v>4</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>48</v>
@@ -6297,7 +6297,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1153</v>
+        <v>1137</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>48</v>
@@ -6449,7 +6449,7 @@
         <v>6</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>48</v>
@@ -6525,7 +6525,7 @@
         <v>5</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1138</v>
+        <v>1164</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>48</v>
@@ -6677,7 +6677,7 @@
         <v>4</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1147</v>
+        <v>1165</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>48</v>
@@ -6791,7 +6791,7 @@
         <v>4</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1145</v>
+        <v>1166</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>143</v>
@@ -6932,7 +6932,7 @@
         <v>3</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1139</v>
+        <v>1167</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>48</v>
@@ -7084,7 +7084,7 @@
         <v>3</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>246</v>
@@ -7160,7 +7160,7 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>246</v>
@@ -7198,7 +7198,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1157</v>
+        <v>1140</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>246</v>
@@ -7303,7 +7303,7 @@
         <v>3</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>1140</v>
+        <v>1168</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>48</v>
@@ -7341,7 +7341,7 @@
         <v>6</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>1148</v>
+        <v>1133</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>48</v>
@@ -7417,7 +7417,7 @@
         <v>3</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>1160</v>
+        <v>1142</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>48</v>
@@ -7493,7 +7493,7 @@
         <v>6</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>48</v>
@@ -7531,7 +7531,7 @@
         <v>5</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>1142</v>
+        <v>1131</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>48</v>
@@ -7922,7 +7922,7 @@
         <v>6</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>48</v>
@@ -8004,7 +8004,7 @@
         <v>48</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>310</v>
@@ -8074,7 +8074,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1146</v>
+        <v>1170</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>48</v>
@@ -8217,7 +8217,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>48</v>
@@ -8436,7 +8436,7 @@
         <v>3</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1161</v>
+        <v>1143</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>48</v>
@@ -8722,7 +8722,7 @@
         <v>5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>48</v>
@@ -8760,7 +8760,7 @@
         <v>6</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1162</v>
+        <v>1144</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>48</v>
@@ -9712,7 +9712,7 @@
         <v>7</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1163</v>
+        <v>1145</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>48</v>
@@ -10331,7 +10331,7 @@
         <v>3</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>1154</v>
+        <v>1138</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>48</v>
@@ -10738,7 +10738,7 @@
         <v>3</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>1155</v>
+        <v>1169</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>48</v>
@@ -10776,7 +10776,7 @@
         <v>7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>48</v>
@@ -10957,7 +10957,7 @@
         <v>6</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>530</v>
@@ -11091,7 +11091,7 @@
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>1170</v>
+        <v>1152</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>56</v>
@@ -11100,7 +11100,7 @@
         <v>4</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>1133</v>
+        <v>1159</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>530</v>
@@ -11757,7 +11757,7 @@
         <v>5</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1134</v>
+        <v>1129</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>530</v>
@@ -12843,7 +12843,7 @@
         <v>3</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1156</v>
+        <v>1139</v>
       </c>
       <c r="E242" s="1" t="s">
         <v>246</v>
@@ -13129,7 +13129,7 @@
         <v>2</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1144</v>
+        <v>1132</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>48</v>
@@ -13167,7 +13167,7 @@
         <v>2</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1165</v>
+        <v>1147</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>48</v>
@@ -15801,7 +15801,7 @@
         <v>0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1116</v>
+        <v>1153</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>48</v>
@@ -16467,7 +16467,7 @@
         <v>0</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>1166</v>
+        <v>1148</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>48</v>
@@ -16505,7 +16505,7 @@
         <v>0</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>1135</v>
+        <v>1130</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>48</v>
@@ -16923,7 +16923,7 @@
         <v>0</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>1164</v>
+        <v>1146</v>
       </c>
       <c r="E355" s="1" t="s">
         <v>48</v>
@@ -17799,7 +17799,7 @@
         <v>0</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1117</v>
+        <v>1156</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>48</v>
@@ -17989,7 +17989,7 @@
         <v>0</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>1111</v>
+        <v>1154</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>48</v>
@@ -18217,7 +18217,7 @@
         <v>0</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E390" s="1" t="s">
         <v>48</v>
@@ -18407,7 +18407,7 @@
         <v>0</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>1118</v>
+        <v>1157</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>48</v>
@@ -18521,7 +18521,7 @@
         <v>0</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1167</v>
+        <v>1149</v>
       </c>
       <c r="E398" s="1" t="s">
         <v>48</v>

</xml_diff>